<commit_message>
Tunning KLI and IDFr
</commit_message>
<xml_diff>
--- a/output/Analysing.xlsx
+++ b/output/Analysing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12647"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12647" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2017 - BM25 Tuning" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
   <si>
     <t>B</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Tuning B parameter in BM25 (Boolean query)</t>
   </si>
   <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t>Title based</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
   </si>
   <si>
     <t>Execution time</t>
-  </si>
-  <si>
-    <t>Execution time:</t>
   </si>
   <si>
     <t>IDF</t>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>Tuning R parameter in KLI (Title based query)</t>
+  </si>
+  <si>
+    <t>BM25 (b=0.0)</t>
   </si>
 </sst>
 </file>
@@ -139,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -171,12 +171,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,16 +196,24 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -996,6 +1013,727 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>2017 IDFr</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (Title based query)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2017 - BM25 Tuning'!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2017 - BM25 Tuning'!$C$24:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2017 - BM25 Tuning'!$C$25:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.09E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.3600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-658E-4787-BE12-F429924FD2A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2021145023"/>
+        <c:axId val="2021149599"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2021145023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2021149599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2021149599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2021145023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>2017 KLI</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (Title based query)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2017 - BM25 Tuning'!$J$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2017 - BM25 Tuning'!$K$24:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2017 - BM25 Tuning'!$K$25:$M$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.6799999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.3399999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1012</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5CF1-4820-90D0-EF3E739FED6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2021145023"/>
+        <c:axId val="2021149599"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2021145023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2021149599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2021149599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2021145023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>2018 training data by B parameter</a:t>
             </a:r>
             <a:br>
@@ -1334,7 +2072,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1707,6 +2445,734 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>2018 IDFr</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (Title based query)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2018 - BM25 Tuning'!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2017 - BM25 Tuning'!$C$24:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2018 - BM25 Tuning'!$C$25:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9AB2-4488-9C58-759018B52A8B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2021145023"/>
+        <c:axId val="2021149599"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2021145023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2021149599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2021149599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2021145023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>2018 KLI</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (Title based query)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2293314272758285"/>
+          <c:y val="3.2992913760457342E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2018 - BM25 Tuning'!$J$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2017 - BM25 Tuning'!$K$24:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2018 - BM25 Tuning'!$K$25:$M$25</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A499-4974-A26B-953DBDB954F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2021145023"/>
+        <c:axId val="2021149599"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2021145023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2021149599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2021149599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2021145023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1867,6 +3333,166 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3377,6 +5003,2018 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3885,13 +7523,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>10583</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>156633</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3915,13 +7553,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>628651</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3938,6 +7576,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>146051</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>628651</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>146051</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4007,6 +7709,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>146051</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>628651</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>146051</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4278,10 +8044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O30"/>
+  <dimension ref="B2:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4290,22 +8056,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="31" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="J2" s="9" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="J2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.5">
       <c r="B3" s="1" t="s">
@@ -4367,7 +8133,7 @@
       <c r="J4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="8">
         <v>0.10879999999999999</v>
       </c>
       <c r="L4" s="3">
@@ -4383,155 +8149,96 @@
         <v>9.6799999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.5">
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3">
-        <v>6.9699999999999998E-2</v>
-      </c>
-      <c r="D5">
-        <v>6.88E-2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>6.7599999999999993E-2</v>
-      </c>
-      <c r="F5" s="3">
-        <v>6.6600000000000006E-2</v>
-      </c>
-      <c r="G5" s="3">
-        <v>6.6299999999999998E-2</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="3">
-        <v>7.1599999999999997E-2</v>
-      </c>
-      <c r="L5" s="11">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="M5" s="3">
-        <v>7.0199999999999999E-2</v>
-      </c>
-      <c r="N5" s="3">
-        <v>6.9500000000000006E-2</v>
-      </c>
-      <c r="O5" s="3">
-        <v>6.9500000000000006E-2</v>
-      </c>
+    <row r="23" spans="2:15" ht="15.7" x14ac:dyDescent="0.5">
+      <c r="B23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="J23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.5">
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.47520000000000001</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.47239999999999999</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.46760000000000002</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.4647</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.46089999999999998</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0.47989999999999999</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0.4773</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0.47160000000000002</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0.4672</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0.46260000000000001</v>
-      </c>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="D24" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="J24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="L24" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="M24" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="N24" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="O24" s="15"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.5">
-      <c r="B24" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="6">
-        <v>2.5694444444444447E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="15.7" x14ac:dyDescent="0.5">
-      <c r="B26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.5">
-      <c r="B27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="D27" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="E27" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.5">
-      <c r="B28" s="3" t="s">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.5">
-      <c r="B29" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.5">
-      <c r="B30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="C25" s="11">
+        <v>8.09E-2</v>
+      </c>
+      <c r="D25" s="3">
+        <v>9.3600000000000003E-2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.1017</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15"/>
+      <c r="J25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" s="11">
+        <v>9.6799999999999997E-2</v>
+      </c>
+      <c r="L25" s="3">
+        <v>9.3399999999999997E-2</v>
+      </c>
+      <c r="M25" s="8">
+        <v>0.1012</v>
+      </c>
+      <c r="N25" s="14"/>
+      <c r="O25" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="N24:O25"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="J2:O2"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="J23:O23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4541,10 +8248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O24"/>
+  <dimension ref="B2:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4553,22 +8260,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="31" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="J2" s="9" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="J2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.5">
       <c r="B3" s="1" t="s">
@@ -4630,7 +8337,7 @@
       <c r="J4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="9">
         <v>0.128</v>
       </c>
       <c r="L4" s="3">
@@ -4722,18 +8429,96 @@
         <v>0.50960000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="6">
-        <v>4.5138888888888888E-2</v>
-      </c>
+    <row r="24" spans="2:15" ht="15.7" x14ac:dyDescent="0.5">
+      <c r="B24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="J24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="D25" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="15"/>
+      <c r="J25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="L25" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="M25" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="N25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="O25" s="15"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0.1123</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.1163</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.12570000000000001</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="G26" s="15"/>
+      <c r="J26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" s="11">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0.1162</v>
+      </c>
+      <c r="M26" s="8">
+        <v>0.12670000000000001</v>
+      </c>
+      <c r="N26" s="14"/>
+      <c r="O26" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="J2:O2"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="F25:G26"/>
+    <mergeCell ref="N25:O26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4759,27 +8544,27 @@
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6">
         <v>0.39930555555555558</v>
@@ -4790,30 +8575,30 @@
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="6">
         <v>0.48819444444444443</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>